<commit_message>
(Uncensored) Added wy2016-17 Combined Outflow fMeHg  folder; Updated fMeHg model results file for wy2016-17; Updated the Combined Outflow Q and WQ worksheet
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_fMeHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_fMeHg Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8F25FF29-0DA4-4998-8DAA-562A3AD843FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8F17AB8-9048-4AAC-8675-97AA0C43046B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="608">
   <si>
     <t>Model #</t>
   </si>
@@ -1344,6 +1344,510 @@
   </si>
   <si>
     <t>Number of Uncensored Observations: 23; Period of record: 2016-01-24 to 2017-04-04</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm1 &lt;- loadReg(fMeHg ~model(1), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 34</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Period of record: 2016-01-20 to 2017-04-26</t>
+  </si>
+  <si>
+    <t>(Intercept)  -8.3936    0.07676 -109.34       0</t>
+  </si>
+  <si>
+    <t>lnQ           0.8435    0.04615   18.28       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1962</t>
+  </si>
+  <si>
+    <t>R-squared: 91.26 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.86 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1792</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3608</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 6.085 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8745</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm2 &lt;- loadReg(fMeHg ~model(2), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm2</t>
+  </si>
+  <si>
+    <t>(Intercept) -8.25827    0.11815 -69.894  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          0.84351    0.04531  18.618  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.04891    0.03290  -1.487  0.1259</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1891</t>
+  </si>
+  <si>
+    <t>R-squared: 91.84 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 85.2 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.241</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2682</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.203 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8544</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm3 &lt;- loadReg(fMeHg ~model(3), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept)  -8.3867    0.07205 -116.409  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           0.8897    0.04764   18.677  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.3885    0.16733   -2.322  0.0196</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1726</t>
+  </si>
+  <si>
+    <t>R-squared: 92.55 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 88.31 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6431</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3077</t>
+  </si>
+  <si>
+    <t>lnQ     1.211</t>
+  </si>
+  <si>
+    <t>DECTIME 1.211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 2.887 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.897</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm4 &lt;- loadReg(fMeHg ~model(4), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -8.5038    0.44131 -19.2693  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           0.8409    0.04729  17.7810  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.3852    0.38256   1.0069  0.2878</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.1542    0.37516  -0.4109  0.6622</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.169</t>
+  </si>
+  <si>
+    <t>R-squared: 92.94 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 90.13 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1562</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2881</t>
+  </si>
+  <si>
+    <t>lnQ         1.219</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.817</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.874</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.972 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.9075</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm5 &lt;- loadReg(fMeHg ~model(5), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm5</t>
+  </si>
+  <si>
+    <t>(Intercept) -8.31198    0.11697 -71.0586  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          0.88385    0.04844  18.2472  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.02733    0.03359  -0.8138  0.3889</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.33920    0.17883  -1.8968  0.0497</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1745</t>
+  </si>
+  <si>
+    <t>R-squared: 92.71 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 89.05 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.764</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2662</t>
+  </si>
+  <si>
+    <t>lnQ     1.239</t>
+  </si>
+  <si>
+    <t>lnQ2    1.130</t>
+  </si>
+  <si>
+    <t>DECTIME 1.368</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 0.7123 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8787</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm6 &lt;- loadReg(fMeHg ~model(6), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm6</t>
+  </si>
+  <si>
+    <t>(Intercept) -8.45278    0.47523 -17.7869  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          0.84162    0.04807  17.5100  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.01164    0.03613  -0.3221  0.7275</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.34997    0.40352   0.8673  0.3508</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.15354    0.38089  -0.4031  0.6629</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1742</t>
+  </si>
+  <si>
+    <t>R-squared: 92.97 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 90.25 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1819</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2748</t>
+  </si>
+  <si>
+    <t>lnQ         1.222</t>
+  </si>
+  <si>
+    <t>lnQ2        1.309</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.127 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8996</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm7 &lt;- loadReg(fMeHg ~model(7), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -7.7987    0.54282 -14.3669  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           0.9240    0.06058  15.2528  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.4349    0.21245  -2.0472  0.0322</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -0.2828    0.48862  -0.5788  0.5320</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.6681    0.43616  -1.5318  0.1039</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1527</t>
+  </si>
+  <si>
+    <t>R-squared: 93.83 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 94.72 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.12</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2622</t>
+  </si>
+  <si>
+    <t>lnQ         2.213</t>
+  </si>
+  <si>
+    <t>DECTIME     2.206</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.888</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.793</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 0.7638 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8979</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm8 &lt;- loadReg(fMeHg ~model(8), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Estimate Std. Error   z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.805408    0.55803 -13.98741  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          0.924611    0.06201  14.91042  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.002986    0.03521   0.08481  0.9255</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.438862    0.22108  -1.98511  0.0344</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.279782    0.49847  -0.56128  0.5374</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.672891    0.44740  -1.50399  0.1041</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1582</t>
+  </si>
+  <si>
+    <t>G-squared: 94.73 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1099</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2644</t>
+  </si>
+  <si>
+    <t>lnQ         2.240</t>
+  </si>
+  <si>
+    <t>lnQ2        1.369</t>
+  </si>
+  <si>
+    <t>DECTIME     2.307</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.924</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.887</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.005 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8994</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm9 &lt;- loadReg(fMeHg ~model(9), data = fMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; fMeHg_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.758351    0.55923 -13.8732  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          0.971725    0.07693  12.6308  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.005235    0.03606  -0.1452  0.8706</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.566703    0.25316  -2.2385  0.0161</t>
+  </si>
+  <si>
+    <t>DECTIME2     1.211466    1.17336   1.0325  0.2512</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.622951    0.59864  -1.0406  0.2476</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.839570    0.47514  -1.7670  0.0537</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1578</t>
+  </si>
+  <si>
+    <t>R-squared: 94.07 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 96.05 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1214</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2344</t>
+  </si>
+  <si>
+    <t>lnQ          3.456</t>
+  </si>
+  <si>
+    <t>lnQ2         1.440</t>
+  </si>
+  <si>
+    <t>DECTIME      3.033</t>
+  </si>
+  <si>
+    <t>DECTIME2     1.943</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 10.009</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  6.656</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.031 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8998</t>
+  </si>
+  <si>
+    <t>&gt; View(fMeHg_Combined)</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34; Period of record: 2016-01-20 to 2017-04-26</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +2075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1675,22 +2179,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1705,7 +2194,25 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2241,8 +2748,8 @@
   <dimension ref="A1:AI68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M29" sqref="M29"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2256,10 +2763,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="6"/>
       <c r="K1" s="21" t="s">
         <v>20</v>
@@ -2298,24 +2805,24 @@
       <c r="L2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="44"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="1:35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
       <c r="Z4" s="18" t="s">
         <v>50</v>
       </c>
@@ -2330,21 +2837,21 @@
       <c r="AI4" s="18"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="36" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="36"/>
+      <c r="L5" s="48"/>
       <c r="Z5" s="18" t="s">
         <v>51</v>
       </c>
@@ -2838,36 +3345,36 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="44"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="45" t="s">
         <v>439</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="36" t="s">
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="36"/>
+      <c r="L18" s="48"/>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -3021,7 +3528,7 @@
       <c r="C22" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="37">
         <v>4.07E-2</v>
       </c>
       <c r="E22" s="35" t="s">
@@ -3354,34 +3861,34 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="36" t="s">
+      <c r="B31" s="45"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="36"/>
+      <c r="L31" s="48"/>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -3746,34 +4253,36 @@
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="44"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="36" t="s">
+      <c r="B44" s="45" t="s">
+        <v>607</v>
+      </c>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="36"/>
+      <c r="L44" s="48"/>
     </row>
     <row r="45" spans="1:27" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -3823,7 +4332,7 @@
       <c r="A46" s="27">
         <v>1</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="6">
         <v>0</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -3841,13 +4350,21 @@
       <c r="G46" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="I46" s="36">
+        <v>91.26</v>
+      </c>
+      <c r="J46" s="36">
+        <v>0.36080000000000001</v>
+      </c>
+      <c r="K46" s="36">
+        <v>6.085</v>
+      </c>
+      <c r="L46" s="36">
+        <v>0.87450000000000006</v>
+      </c>
       <c r="M46" s="27"/>
       <c r="N46" s="8" t="s">
         <v>16</v>
@@ -3863,10 +4380,12 @@
       <c r="A47" s="27">
         <v>2</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="6">
         <v>0</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="25">
+        <v>0.12590000000000001</v>
+      </c>
       <c r="D47" s="10" t="s">
         <v>15</v>
       </c>
@@ -3879,13 +4398,21 @@
       <c r="G47" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
+      <c r="I47" s="36">
+        <v>91.84</v>
+      </c>
+      <c r="J47" s="36">
+        <v>0.26819999999999999</v>
+      </c>
+      <c r="K47" s="36">
+        <v>1.2030000000000001</v>
+      </c>
+      <c r="L47" s="36">
+        <v>0.85440000000000005</v>
+      </c>
       <c r="M47" s="27"/>
       <c r="N47" s="8" t="s">
         <v>16</v>
@@ -3898,33 +4425,45 @@
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A48" s="27">
+      <c r="A48" s="11">
         <v>3</v>
       </c>
       <c r="B48" s="11">
         <v>0</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="10" t="s">
+      <c r="D48" s="37">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="E48" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="35" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
+      <c r="I48" s="11">
+        <v>92.55</v>
+      </c>
+      <c r="J48" s="11">
+        <v>0.30769999999999997</v>
+      </c>
+      <c r="K48" s="11">
+        <v>2.887</v>
+      </c>
+      <c r="L48" s="36">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>269</v>
+      </c>
       <c r="N48" s="8" t="s">
         <v>16</v>
       </c>
@@ -3939,7 +4478,7 @@
       <c r="A49" s="27">
         <v>4</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="6">
         <v>0</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -3951,15 +4490,27 @@
       <c r="E49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="11" t="s">
+      <c r="F49" s="6">
+        <v>0.2878</v>
+      </c>
+      <c r="G49" s="36">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
+      <c r="I49" s="36">
+        <v>92.94</v>
+      </c>
+      <c r="J49" s="36">
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="K49" s="36">
+        <v>1.972</v>
+      </c>
+      <c r="L49" s="36">
+        <v>0.90749999999999997</v>
+      </c>
       <c r="M49" s="27"/>
       <c r="N49" s="8" t="s">
         <v>16</v>
@@ -3975,11 +4526,15 @@
       <c r="A50" s="27">
         <v>5</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="6">
         <v>0</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="36">
+        <v>0.38890000000000002</v>
+      </c>
+      <c r="D50" s="36">
+        <v>4.9700000000000001E-2</v>
+      </c>
       <c r="E50" s="10" t="s">
         <v>15</v>
       </c>
@@ -3989,13 +4544,21 @@
       <c r="G50" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="H50" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
+      <c r="I50" s="36">
+        <v>92.71</v>
+      </c>
+      <c r="J50" s="36">
+        <v>0.26619999999999999</v>
+      </c>
+      <c r="K50" s="36">
+        <v>0.71230000000000004</v>
+      </c>
+      <c r="L50" s="36">
+        <v>0.87870000000000004</v>
+      </c>
       <c r="M50" s="27"/>
       <c r="N50" s="8" t="s">
         <v>16</v>
@@ -4011,25 +4574,39 @@
       <c r="A51" s="27">
         <v>6</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="6">
         <v>0</v>
       </c>
-      <c r="C51" s="27"/>
+      <c r="C51" s="36">
+        <v>0.72750000000000004</v>
+      </c>
       <c r="D51" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="11" t="s">
+      <c r="F51" s="6">
+        <v>0.3508</v>
+      </c>
+      <c r="G51" s="36">
+        <v>0.66290000000000004</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
+      <c r="I51" s="36">
+        <v>92.97</v>
+      </c>
+      <c r="J51" s="36">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="K51" s="36">
+        <v>1.127</v>
+      </c>
+      <c r="L51" s="36">
+        <v>0.89959999999999996</v>
+      </c>
       <c r="M51" s="27"/>
       <c r="N51" s="8" t="s">
         <v>16</v>
@@ -4045,25 +4622,39 @@
       <c r="A52" s="27">
         <v>7</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="6">
         <v>0</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6">
+        <v>3.2199999999999999E-2</v>
+      </c>
       <c r="E52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="11" t="s">
+      <c r="F52" s="6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="G52" s="36">
+        <v>0.10390000000000001</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
+      <c r="I52" s="36">
+        <v>93.83</v>
+      </c>
+      <c r="J52" s="36">
+        <v>0.26219999999999999</v>
+      </c>
+      <c r="K52" s="36">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="L52" s="36">
+        <v>0.89790000000000003</v>
+      </c>
       <c r="M52" s="27"/>
       <c r="N52" s="8" t="s">
         <v>16</v>
@@ -4079,23 +4670,39 @@
       <c r="A53" s="27">
         <v>8</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="6">
         <v>0</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="36">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="D53" s="6">
+        <v>3.44E-2</v>
+      </c>
       <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="11" t="s">
+      <c r="F53" s="6">
+        <v>0.53739999999999999</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.1041</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-      <c r="L53" s="27"/>
+      <c r="I53" s="36">
+        <v>93.83</v>
+      </c>
+      <c r="J53" s="36">
+        <v>0.26440000000000002</v>
+      </c>
+      <c r="K53" s="36">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="L53" s="36">
+        <v>0.89939999999999998</v>
+      </c>
       <c r="M53" s="27"/>
       <c r="N53" s="8" t="s">
         <v>16</v>
@@ -4111,21 +4718,39 @@
       <c r="A54" s="27">
         <v>9</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="6">
         <v>0</v>
       </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="11" t="s">
+      <c r="C54" s="36">
+        <v>0.87060000000000004</v>
+      </c>
+      <c r="D54" s="6">
+        <v>1.61E-2</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0.25119999999999998</v>
+      </c>
+      <c r="F54" s="6">
+        <v>0.24759999999999999</v>
+      </c>
+      <c r="G54" s="6">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
+      <c r="I54" s="36">
+        <v>94.07</v>
+      </c>
+      <c r="J54" s="36">
+        <v>0.2344</v>
+      </c>
+      <c r="K54" s="36">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="L54" s="36">
+        <v>0.89980000000000004</v>
+      </c>
       <c r="M54" s="27"/>
       <c r="N54" s="8" t="s">
         <v>16</v>
@@ -4143,34 +4768,34 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
-      <c r="J57" s="42"/>
-      <c r="K57" s="36"/>
-      <c r="L57" s="36"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="48"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="37"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="36" t="s">
+      <c r="B58" s="45"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="47"/>
+      <c r="K58" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="36"/>
+      <c r="L58" s="48"/>
     </row>
     <row r="59" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -4410,12 +5035,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K58:L58"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="B18:J18"/>
@@ -4428,6 +5047,12 @@
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="K44:L44"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <conditionalFormatting sqref="L60:L68 L57 L93:L1048576">
     <cfRule type="cellIs" dxfId="17" priority="42" operator="between">
@@ -11008,118 +11633,176 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FBE2AD-EC1E-4563-8289-C8C08DD23DD5}">
-  <dimension ref="A1:A528"/>
+  <dimension ref="A1:A529"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="14" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="14" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -11128,1477 +11811,2294 @@
       <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="15" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="14" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="14" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="14" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="14" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="14" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="14" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="14" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="14" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="14" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="14" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="15" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="14" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="14" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="14" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="14" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="14" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="14" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="14" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
+      <c r="A145" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
+      <c r="A146" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="14" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="14" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="14" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="14" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="15" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="15" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
+      <c r="A176" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
+      <c r="A177" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="14" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="14" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="14" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="14" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="14" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="14" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
+      <c r="A205" s="14" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
+      <c r="A214" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="14" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="14" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="14" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="15"/>
+      <c r="A222" s="15" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="15"/>
+      <c r="A226" s="15" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="14"/>
+      <c r="A229" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="14"/>
+      <c r="A230" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
+      <c r="A232" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
+      <c r="A234" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="14" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="14" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
+      <c r="A246" s="14" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="14" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="14" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="14" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
+      <c r="A252" s="14" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="14" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="14" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
+      <c r="A257" s="14" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="14" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="14" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="14" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
+      <c r="A267" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
+      <c r="A275" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="14" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="14" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="14" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="15"/>
+      <c r="A280" s="15" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="15"/>
+      <c r="A284" s="15" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
+      <c r="A287" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="14" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="14" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="14" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="14" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="14" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="14" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="14" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="14" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="14"/>
+      <c r="A312" s="14" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="14"/>
+      <c r="A313" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="14"/>
+      <c r="A314" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="14"/>
+      <c r="A315" s="14" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="14"/>
+      <c r="A316" s="14" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="14" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="14" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="14" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="14" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="14" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="14"/>
+      <c r="A327" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="14" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="14" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="14" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15"/>
+      <c r="A340" s="15" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+      <c r="A342" s="7" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+      <c r="A343" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="15"/>
+      <c r="A344" s="15" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
+      <c r="A351" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
+      <c r="A352" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+      <c r="A353" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="14"/>
+      <c r="A354" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
+      <c r="A356" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
+      <c r="A357" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
+      <c r="A359" s="14" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
+      <c r="A361" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
+      <c r="A362" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="14" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="14" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="14" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
+      <c r="A366" s="14" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
+      <c r="A367" s="14" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
+      <c r="A369" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="14" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="14" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="14" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="14" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="14" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="14" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="14" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="14" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="14" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="14" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="14" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="14" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="14"/>
+      <c r="A398" s="14" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="15"/>
+      <c r="A400" s="15" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+      <c r="A401" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+      <c r="A402" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+      <c r="A403" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="15"/>
+      <c r="A404" s="15" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="14"/>
+      <c r="A411" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="14"/>
+      <c r="A417" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="14"/>
+      <c r="A419" s="14" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="14"/>
+      <c r="A421" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="14"/>
+      <c r="A422" s="14" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="14"/>
+      <c r="A423" s="14" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="14"/>
+      <c r="A424" s="14" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="14"/>
+      <c r="A425" s="14" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="14"/>
+      <c r="A426" s="14" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="14"/>
+      <c r="A427" s="14" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="14"/>
+      <c r="A428" s="14" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="14"/>
+      <c r="A430" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="14"/>
+      <c r="A431" s="14" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
+      <c r="A432" s="14" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
+      <c r="A433" s="14" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
+      <c r="A434" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
+      <c r="A435" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
+      <c r="A436" s="14" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="14"/>
+      <c r="A437" s="14" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="14"/>
+      <c r="A438" s="14" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="14"/>
+      <c r="A440" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
+      <c r="A441" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="14"/>
+      <c r="A442" s="14" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="14"/>
+      <c r="A443" s="14" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="14"/>
+      <c r="A444" s="14" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
+      <c r="A445" s="14" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
+      <c r="A446" s="14" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="14"/>
+      <c r="A456" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="14"/>
+      <c r="A457" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
+      <c r="A458" s="14" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
+      <c r="A459" s="14" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="14"/>
+      <c r="A460" s="14" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="15"/>
+      <c r="A462" s="15" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="15"/>
+      <c r="A466" s="15" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="14"/>
+      <c r="A467" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="14"/>
+      <c r="A469" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="14"/>
+      <c r="A470" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="14"/>
+      <c r="A472" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="14"/>
+      <c r="A473" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="14"/>
+      <c r="A474" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="14"/>
+      <c r="A475" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="14"/>
+      <c r="A476" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="14"/>
+      <c r="A478" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="14"/>
+      <c r="A479" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="14"/>
+      <c r="A481" s="14" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="14"/>
+      <c r="A483" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="14"/>
+      <c r="A484" s="14" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="14"/>
+      <c r="A485" s="14" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="14"/>
+      <c r="A486" s="14" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="14"/>
+      <c r="A487" s="14" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="14"/>
+      <c r="A488" s="14" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="14"/>
+      <c r="A489" s="14" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="14"/>
+      <c r="A490" s="14" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="14"/>
+      <c r="A491" s="14" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="14"/>
+      <c r="A493" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="14"/>
+      <c r="A494" s="14" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="14"/>
+      <c r="A495" s="14" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="14"/>
+      <c r="A496" s="14" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="14"/>
+      <c r="A497" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="14"/>
+      <c r="A498" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="14"/>
+      <c r="A499" s="14" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="14"/>
+      <c r="A500" s="14" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" s="14"/>
+      <c r="A501" s="14" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" s="14"/>
+      <c r="A503" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" s="14"/>
+      <c r="A504" s="14" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="14"/>
+      <c r="A505" s="14" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" s="14"/>
+      <c r="A506" s="14" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" s="14"/>
+      <c r="A507" s="14" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" s="14"/>
+      <c r="A508" s="14" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" s="14"/>
+      <c r="A509" s="14" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" s="14"/>
+      <c r="A510" s="14" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" s="14"/>
+      <c r="A512" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" s="14"/>
+      <c r="A513" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" s="14"/>
+      <c r="A514" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" s="14"/>
+      <c r="A515" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" s="14"/>
+      <c r="A516" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="14"/>
+      <c r="A517" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="14"/>
+      <c r="A518" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" s="14"/>
+      <c r="A520" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="14"/>
+      <c r="A521" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="14"/>
+      <c r="A522" s="14" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="14"/>
+      <c r="A523" s="14" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" s="14"/>
+      <c r="A524" s="14" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A525" s="16"/>
+      <c r="A525" s="13"/>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A526" s="16"/>
+      <c r="A526" s="15" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A527" s="17"/>
+      <c r="A527" s="16"/>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A528" s="12"/>
+      <c r="A528" s="17"/>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
***FOUND ERROR IN MODEL RESULTS*** Reloaded Rumsey wy2016-17 pMeHg, fMeHg, and wwMeHg folders; reloaded the 3 model stats for MeHg, reloaded the files for Sigma Plot PDFs and Powerpoint files.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_fMeHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_fMeHg Model Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E3462-66AD-41DE-8023-5DE1FCBA4AD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B035BC6-B7FD-4828-988B-E94D58D9C585}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fMeHg wy2016-17 Model Results" sheetId="2" r:id="rId1"/>
@@ -3015,19 +3015,19 @@
     <t>Number of Uncensored Observations: 40; Period of record: 2015-12-19 to 2017-05-15</t>
   </si>
   <si>
-    <t>1,228; 1,249</t>
-  </si>
-  <si>
-    <t>1092; 1285</t>
-  </si>
-  <si>
-    <t>215, 388</t>
-  </si>
-  <si>
-    <t>227, 414</t>
-  </si>
-  <si>
-    <t>145, 300</t>
+    <t>8.14, 8.01</t>
+  </si>
+  <si>
+    <t>9.16, 7.78</t>
+  </si>
+  <si>
+    <t>46.47, 25.78</t>
+  </si>
+  <si>
+    <t>44.02, 24.16</t>
+  </si>
+  <si>
+    <t>69.08, 33.29</t>
   </si>
 </sst>
 </file>
@@ -3297,7 +3297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3442,19 +3442,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3475,7 +3463,22 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4031,8 +4034,8 @@
   <dimension ref="A1:AL70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P79" sqref="P79:P80"/>
+      <pane ySplit="4" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4060,17 +4063,17 @@
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="57"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
       <c r="L1" s="42"/>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="58"/>
+      <c r="N1" s="65"/>
       <c r="P1" s="36"/>
       <c r="Q1" s="2"/>
     </row>
@@ -4199,18 +4202,18 @@
       <c r="O5" s="37"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
       <c r="AC6" s="18" t="s">
         <v>48</v>
       </c>
@@ -4225,22 +4228,22 @@
       <c r="AL6" s="18"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="58" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="54" t="s">
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="54"/>
+      <c r="M7" s="61"/>
       <c r="AC7" s="18" t="s">
         <v>49</v>
       </c>
@@ -4766,38 +4769,38 @@
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="61"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="58" t="s">
         <v>425</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="54" t="s">
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="54"/>
+      <c r="M20" s="61"/>
     </row>
     <row r="21" spans="1:28" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -5321,38 +5324,38 @@
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="61"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="57"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="58" t="s">
         <v>771</v>
       </c>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="54" t="s">
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="M33" s="54"/>
+      <c r="M33" s="61"/>
     </row>
     <row r="34" spans="1:28" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
@@ -5860,38 +5863,38 @@
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="61"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="57"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="58" t="s">
         <v>593</v>
       </c>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="54" t="s">
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="60"/>
+      <c r="L46" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="M46" s="54"/>
+      <c r="M46" s="61"/>
     </row>
     <row r="47" spans="1:28" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
@@ -6401,38 +6404,38 @@
       <c r="AB57" s="9"/>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B59" s="59" t="s">
+      <c r="B59" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="60"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="60"/>
-      <c r="K59" s="61"/>
-      <c r="L59" s="54"/>
-      <c r="M59" s="54"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="56"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="61"/>
+      <c r="M59" s="61"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B60" s="62" t="s">
+      <c r="B60" s="58" t="s">
         <v>979</v>
       </c>
-      <c r="C60" s="63"/>
-      <c r="D60" s="63"/>
-      <c r="E60" s="63"/>
-      <c r="F60" s="63"/>
-      <c r="G60" s="63"/>
-      <c r="H60" s="63"/>
-      <c r="I60" s="63"/>
-      <c r="J60" s="63"/>
-      <c r="K60" s="64"/>
-      <c r="L60" s="54" t="s">
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="60"/>
+      <c r="L60" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="M60" s="54"/>
+      <c r="M60" s="61"/>
     </row>
     <row r="61" spans="1:28" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
@@ -6488,7 +6491,7 @@
       </c>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+      <c r="A62" s="6">
         <v>1</v>
       </c>
       <c r="B62" s="6">
@@ -6512,27 +6515,28 @@
       <c r="H62" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I62" s="53">
+      <c r="I62" s="6">
         <v>92.73</v>
       </c>
-      <c r="J62" s="53">
+      <c r="J62" s="6">
         <v>0.75970000000000004</v>
       </c>
-      <c r="K62" s="53">
+      <c r="K62" s="6">
         <v>0.42759999999999998</v>
       </c>
-      <c r="L62" s="53">
+      <c r="L62" s="6">
         <v>7.7069999999999999</v>
       </c>
       <c r="M62" s="53">
         <v>0.80400000000000005</v>
       </c>
-      <c r="N62" s="1" t="s">
+      <c r="N62" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="O62" s="65" t="s">
+      <c r="O62" s="66" t="s">
         <v>980</v>
       </c>
+      <c r="P62" s="54"/>
       <c r="Q62" s="8" t="s">
         <v>16</v>
       </c>
@@ -6544,50 +6548,53 @@
       </c>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+      <c r="A63" s="11">
         <v>2</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="11">
         <v>0</v>
       </c>
-      <c r="C63" s="22">
+      <c r="C63" s="34">
         <v>2.9499999999999998E-2</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G63" s="10" t="s">
+      <c r="G63" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="6" t="s">
+      <c r="H63" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I63" s="53">
+      <c r="I63" s="11">
         <v>93.55</v>
       </c>
-      <c r="J63" s="53">
+      <c r="J63" s="11">
         <v>0.56069999999999998</v>
       </c>
-      <c r="K63" s="53">
+      <c r="K63" s="11">
         <v>0.37</v>
       </c>
-      <c r="L63" s="53">
+      <c r="L63" s="11">
         <v>-0.76529999999999998</v>
       </c>
       <c r="M63" s="53">
         <v>0.81540000000000001</v>
       </c>
-      <c r="N63" s="1" t="s">
+      <c r="N63" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="O63" s="36" t="s">
+      <c r="O63" s="39" t="s">
         <v>981</v>
+      </c>
+      <c r="P63" s="39" t="s">
+        <v>776</v>
       </c>
       <c r="Q63" s="8" t="s">
         <v>16</v>
@@ -6812,54 +6819,52 @@
       </c>
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A68" s="11">
+      <c r="A68" s="6">
         <v>7</v>
       </c>
-      <c r="B68" s="11">
+      <c r="B68" s="6">
         <v>0</v>
       </c>
-      <c r="C68" s="32" t="s">
+      <c r="C68" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D68" s="11">
+      <c r="D68" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E68" s="32" t="s">
+      <c r="E68" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F68" s="11">
+      <c r="F68" s="6">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="G68" s="11">
+      <c r="G68" s="6">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="H68" s="11" t="s">
+      <c r="H68" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I68" s="11">
+      <c r="I68" s="6">
         <v>94.91</v>
       </c>
-      <c r="J68" s="11">
+      <c r="J68" s="6">
         <v>0.80840000000000001</v>
       </c>
-      <c r="K68" s="11">
+      <c r="K68" s="6">
         <v>0.24129999999999999</v>
       </c>
-      <c r="L68" s="11">
+      <c r="L68" s="6">
         <v>3.3050000000000002</v>
       </c>
       <c r="M68" s="53">
         <v>0.90290000000000004</v>
       </c>
-      <c r="N68" s="39" t="s">
+      <c r="N68" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="O68" s="39" t="s">
+      <c r="O68" s="54" t="s">
         <v>984</v>
       </c>
-      <c r="P68" s="39" t="s">
-        <v>255</v>
-      </c>
+      <c r="P68" s="54"/>
       <c r="Q68" s="8" t="s">
         <v>16</v>
       </c>
@@ -6972,12 +6977,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B19:K19"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="M1:N1"/>
     <mergeCell ref="L60:M60"/>
     <mergeCell ref="B60:K60"/>
     <mergeCell ref="B20:K20"/>
@@ -6990,6 +6989,12 @@
     <mergeCell ref="L33:M33"/>
     <mergeCell ref="B45:K45"/>
     <mergeCell ref="L46:M46"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="M62:M70 M59 M95:M1048576">
     <cfRule type="cellIs" dxfId="19" priority="44" operator="between">

</xml_diff>